<commit_message>
MSX0 Octopus → MSX0 Booster
名前を修正
</commit_message>
<xml_diff>
--- a/msx3gen/files/msx_gen3.xlsx
+++ b/msx3gen/files/msx_gen3.xlsx
@@ -1627,10 +1627,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>MSX0 Octopus</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>なし？</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -1699,6 +1695,10 @@
     <rPh sb="6" eb="8">
       <t>リヨウ</t>
     </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>MSX0 Booster</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -3229,10 +3229,10 @@
   <dimension ref="A3:X66"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="4" ySplit="7" topLeftCell="L8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="7" topLeftCell="O8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="N17" sqref="N17"/>
+      <selection pane="bottomRight" activeCell="Z14" sqref="Z14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -3873,40 +3873,40 @@
         <v>235</v>
       </c>
       <c r="D16" s="84" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="E16" s="97" t="s">
         <v>183</v>
       </c>
       <c r="F16" s="30" t="s">
+        <v>236</v>
+      </c>
+      <c r="G16" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="G16" s="1" t="s">
+      <c r="H16" s="30" t="s">
         <v>238</v>
       </c>
-      <c r="H16" s="30" t="s">
+      <c r="I16" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="I16" s="1" t="s">
+      <c r="J16" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="L16" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="M16" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="N16" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="O16" s="30" t="s">
         <v>240</v>
-      </c>
-      <c r="J16" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="K16" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="L16" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="M16" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="N16" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="O16" s="30" t="s">
-        <v>241</v>
       </c>
       <c r="P16" s="86" t="s">
         <v>33</v>
@@ -3921,7 +3921,7 @@
         <v>166</v>
       </c>
       <c r="T16" s="30" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="U16" s="1" t="s">
         <v>165</v>

</xml_diff>

<commit_message>
Booster を Booster0 と Booster3 に分離
</commit_message>
<xml_diff>
--- a/msx3gen/files/msx_gen3.xlsx
+++ b/msx3gen/files/msx_gen3.xlsx
@@ -12,7 +12,7 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="23310" windowHeight="6915"/>
   </bookViews>
   <sheets>
-    <sheet name="2024年9月30日" sheetId="8" r:id="rId1"/>
+    <sheet name="2024年10月12日" sheetId="8" r:id="rId1"/>
     <sheet name="2024年9月29日" sheetId="7" r:id="rId2"/>
     <sheet name="2024年9月28日 ver4" sheetId="6" r:id="rId3"/>
     <sheet name="2024年9月28日 ver3" sheetId="5" r:id="rId4"/>
@@ -22,11 +22,11 @@
     <sheet name="2024年9月25日 ver" sheetId="1" r:id="rId8"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'2024年10月12日'!$A$1:$Y$58</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="4">'2024年9月28日 ver2'!$A$1:$W$50</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="3">'2024年9月28日 ver3'!$A$1:$W$51</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="2">'2024年9月28日 ver4'!$A$1:$Z$48</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">'2024年9月29日'!$A$1:$Y$55</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'2024年9月30日'!$A$1:$Y$57</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -43,7 +43,7 @@
     <author>Takayuki Hara</author>
   </authors>
   <commentList>
-    <comment ref="E19" authorId="0" shapeId="0">
+    <comment ref="E20" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -60,7 +60,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E20" authorId="0" shapeId="0">
+    <comment ref="E21" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -170,7 +170,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3138" uniqueCount="247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3162" uniqueCount="254">
   <si>
     <t>旧来のMSX</t>
     <rPh sb="0" eb="2">
@@ -1652,19 +1652,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>MSX0 Octopus 自体が
-カートリッジ。
-MSXのカートリッジスロット
-に装着する。</t>
-    <rPh sb="13" eb="15">
-      <t>ジタイ</t>
-    </rPh>
-    <rPh sb="41" eb="43">
-      <t>ソウチャク</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>搭載する USB/I2C の
 数を再検討中</t>
     <rPh sb="0" eb="2">
@@ -1698,10 +1685,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>MSX0 Booster</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>(12)</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -1717,6 +1700,80 @@
   </si>
   <si>
     <t>https://x.com/nishikazuhiko/status/1695967501975466424</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>MSX0 Booster0</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>MSX0 Booster3</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>MSX0 Booster0 自体が
+カートリッジ。
+MSXのカートリッジスロット
+に装着する。</t>
+    <rPh sb="14" eb="16">
+      <t>ジタイ</t>
+    </rPh>
+    <rPh sb="42" eb="44">
+      <t>ソウチャク</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>MSX0 Booster3 自体が
+カートリッジ。
+MSXのカートリッジスロット
+に装着する。</t>
+    <rPh sb="14" eb="16">
+      <t>ジタイ</t>
+    </rPh>
+    <rPh sb="42" eb="44">
+      <t>ソウチャク</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>???</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>搭載する USB/I2C の
+数を再検討中
+MSX engine3 を追加すれば、booster3 へアップグレード可能</t>
+    <rPh sb="0" eb="2">
+      <t>トウサイ</t>
+    </rPh>
+    <rPh sb="15" eb="16">
+      <t>カズ</t>
+    </rPh>
+    <rPh sb="17" eb="20">
+      <t>サイケントウ</t>
+    </rPh>
+    <rPh sb="20" eb="21">
+      <t>チュウ</t>
+    </rPh>
+    <rPh sb="35" eb="37">
+      <t>ツイカ</t>
+    </rPh>
+    <rPh sb="58" eb="60">
+      <t>カノウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">(13) </t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>MSX0 Booster0 と Booster3</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>https://x.com/nishikazuhiko/status/1695642892734521625</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -3244,13 +3301,13 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A3:X69"/>
+  <dimension ref="A3:X73"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="7" topLeftCell="E21" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="7" topLeftCell="Q42" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="B70" sqref="B70"/>
+      <selection pane="bottomRight" activeCell="R71" sqref="R71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -3885,13 +3942,13 @@
       </c>
       <c r="X15" s="3"/>
     </row>
-    <row r="16" spans="2:24" ht="54">
+    <row r="16" spans="2:24" ht="67.5">
       <c r="B16" s="108"/>
       <c r="C16" s="102" t="s">
         <v>235</v>
       </c>
       <c r="D16" s="84" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="E16" s="97" t="s">
         <v>183</v>
@@ -3900,13 +3957,13 @@
         <v>236</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>237</v>
+        <v>142</v>
       </c>
       <c r="H16" s="30" t="s">
         <v>238</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>239</v>
+        <v>167</v>
       </c>
       <c r="J16" s="1" t="s">
         <v>42</v>
@@ -3921,10 +3978,10 @@
         <v>42</v>
       </c>
       <c r="N16" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="O16" s="30" t="s">
-        <v>240</v>
+        <v>247</v>
       </c>
       <c r="P16" s="86" t="s">
         <v>33</v>
@@ -3939,7 +3996,7 @@
         <v>166</v>
       </c>
       <c r="T16" s="30" t="s">
-        <v>241</v>
+        <v>250</v>
       </c>
       <c r="U16" s="1" t="s">
         <v>165</v>
@@ -3952,28 +4009,28 @@
       </c>
       <c r="X16" s="3"/>
     </row>
-    <row r="17" spans="1:24" ht="54">
+    <row r="17" spans="2:24" ht="54">
       <c r="B17" s="108"/>
-      <c r="C17" s="92" t="s">
-        <v>69</v>
+      <c r="C17" s="102" t="s">
+        <v>235</v>
       </c>
       <c r="D17" s="84" t="s">
-        <v>206</v>
-      </c>
-      <c r="E17" s="96" t="s">
-        <v>187</v>
+        <v>246</v>
+      </c>
+      <c r="E17" s="97" t="s">
+        <v>183</v>
       </c>
       <c r="F17" s="30" t="s">
-        <v>20</v>
+        <v>236</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>30</v>
+        <v>237</v>
       </c>
       <c r="H17" s="30" t="s">
-        <v>56</v>
+        <v>249</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>37</v>
+        <v>239</v>
       </c>
       <c r="J17" s="1" t="s">
         <v>42</v>
@@ -3985,29 +4042,31 @@
         <v>42</v>
       </c>
       <c r="M17" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="N17" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="O17" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="P17" s="104" t="s">
-        <v>208</v>
+        <v>241</v>
+      </c>
+      <c r="O17" s="30" t="s">
+        <v>248</v>
+      </c>
+      <c r="P17" s="86" t="s">
+        <v>33</v>
       </c>
       <c r="Q17" s="1" t="s">
         <v>39</v>
       </c>
       <c r="R17" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="S17" s="30" t="s">
-        <v>234</v>
-      </c>
-      <c r="T17" s="1"/>
+        <v>70</v>
+      </c>
+      <c r="S17" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="T17" s="30" t="s">
+        <v>240</v>
+      </c>
       <c r="U17" s="1" t="s">
-        <v>117</v>
+        <v>165</v>
       </c>
       <c r="V17" s="86" t="s">
         <v>163</v>
@@ -4017,25 +4076,25 @@
       </c>
       <c r="X17" s="3"/>
     </row>
-    <row r="18" spans="1:24" ht="54">
+    <row r="18" spans="2:24" ht="54">
       <c r="B18" s="108"/>
       <c r="C18" s="92" t="s">
-        <v>198</v>
+        <v>69</v>
       </c>
       <c r="D18" s="84" t="s">
-        <v>10</v>
+        <v>206</v>
       </c>
       <c r="E18" s="96" t="s">
-        <v>188</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>18</v>
+        <v>187</v>
+      </c>
+      <c r="F18" s="30" t="s">
+        <v>20</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="H18" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
+      </c>
+      <c r="H18" s="30" t="s">
+        <v>56</v>
       </c>
       <c r="I18" s="1" t="s">
         <v>37</v>
@@ -4044,71 +4103,69 @@
         <v>42</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="L18" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="M18" s="1" t="s">
         <v>45</v>
       </c>
       <c r="N18" s="1" t="s">
-        <v>106</v>
+        <v>52</v>
       </c>
       <c r="O18" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="P18" s="86" t="s">
-        <v>180</v>
+        <v>39</v>
+      </c>
+      <c r="P18" s="104" t="s">
+        <v>208</v>
       </c>
       <c r="Q18" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="R18" s="30" t="s">
-        <v>220</v>
+        <v>39</v>
+      </c>
+      <c r="R18" s="1" t="s">
+        <v>164</v>
       </c>
       <c r="S18" s="30" t="s">
-        <v>209</v>
-      </c>
-      <c r="T18" s="30" t="s">
-        <v>211</v>
-      </c>
+        <v>234</v>
+      </c>
+      <c r="T18" s="1"/>
       <c r="U18" s="1" t="s">
         <v>117</v>
       </c>
       <c r="V18" s="86" t="s">
-        <v>144</v>
+        <v>163</v>
       </c>
       <c r="W18" s="1" t="s">
         <v>128</v>
       </c>
       <c r="X18" s="3"/>
     </row>
-    <row r="19" spans="1:24" ht="51.75">
+    <row r="19" spans="2:24" ht="54">
       <c r="B19" s="108"/>
       <c r="C19" s="92" t="s">
         <v>198</v>
       </c>
       <c r="D19" s="84" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="E19" s="96" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>18</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>151</v>
+        <v>27</v>
       </c>
       <c r="I19" s="1" t="s">
         <v>37</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="K19" s="1" t="s">
         <v>45</v>
@@ -4131,8 +4188,8 @@
       <c r="Q19" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="R19" s="1" t="s">
-        <v>73</v>
+      <c r="R19" s="30" t="s">
+        <v>220</v>
       </c>
       <c r="S19" s="30" t="s">
         <v>209</v>
@@ -4141,23 +4198,23 @@
         <v>211</v>
       </c>
       <c r="U19" s="1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="V19" s="86" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="W19" s="1" t="s">
         <v>128</v>
       </c>
       <c r="X19" s="3"/>
     </row>
-    <row r="20" spans="1:24" ht="51.75">
+    <row r="20" spans="2:24" ht="51.75">
       <c r="B20" s="108"/>
       <c r="C20" s="92" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="D20" s="84" t="s">
-        <v>199</v>
+        <v>3</v>
       </c>
       <c r="E20" s="96" t="s">
         <v>189</v>
@@ -4218,34 +4275,34 @@
       </c>
       <c r="X20" s="3"/>
     </row>
-    <row r="21" spans="1:24" ht="54">
+    <row r="21" spans="2:24" ht="51.75">
       <c r="B21" s="108"/>
       <c r="C21" s="92" t="s">
-        <v>198</v>
+        <v>204</v>
       </c>
       <c r="D21" s="84" t="s">
-        <v>58</v>
+        <v>199</v>
       </c>
       <c r="E21" s="96" t="s">
-        <v>190</v>
-      </c>
-      <c r="F21" s="30" t="s">
-        <v>61</v>
-      </c>
-      <c r="G21" s="86" t="s">
-        <v>62</v>
-      </c>
-      <c r="H21" s="30" t="s">
-        <v>152</v>
+        <v>189</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>151</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="J21" s="30" t="s">
-        <v>45</v>
-      </c>
-      <c r="K21" s="86" t="s">
-        <v>46</v>
+        <v>37</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="K21" s="1" t="s">
+        <v>45</v>
       </c>
       <c r="L21" s="1" t="s">
         <v>44</v>
@@ -4254,7 +4311,7 @@
         <v>45</v>
       </c>
       <c r="N21" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="O21" s="1" t="s">
         <v>45</v>
@@ -4263,10 +4320,10 @@
         <v>180</v>
       </c>
       <c r="Q21" s="1" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="R21" s="1" t="s">
-        <v>109</v>
+        <v>73</v>
       </c>
       <c r="S21" s="30" t="s">
         <v>209</v>
@@ -4278,32 +4335,32 @@
         <v>116</v>
       </c>
       <c r="V21" s="86" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="W21" s="1" t="s">
         <v>128</v>
       </c>
       <c r="X21" s="3"/>
     </row>
-    <row r="22" spans="1:24" ht="54">
+    <row r="22" spans="2:24" ht="54">
       <c r="B22" s="108"/>
       <c r="C22" s="92" t="s">
         <v>198</v>
       </c>
       <c r="D22" s="84" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E22" s="96" t="s">
         <v>190</v>
       </c>
       <c r="F22" s="30" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="G22" s="86" t="s">
-        <v>33</v>
+        <v>62</v>
       </c>
       <c r="H22" s="30" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="I22" s="1" t="s">
         <v>90</v>
@@ -4333,7 +4390,7 @@
         <v>39</v>
       </c>
       <c r="R22" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="S22" s="30" t="s">
         <v>209</v>
@@ -4345,50 +4402,50 @@
         <v>116</v>
       </c>
       <c r="V22" s="86" t="s">
-        <v>33</v>
+        <v>145</v>
       </c>
       <c r="W22" s="1" t="s">
         <v>128</v>
       </c>
       <c r="X22" s="3"/>
     </row>
-    <row r="23" spans="1:24" ht="94.5">
+    <row r="23" spans="2:24" ht="54">
       <c r="B23" s="108"/>
       <c r="C23" s="92" t="s">
         <v>198</v>
       </c>
       <c r="D23" s="84" t="s">
-        <v>12</v>
+        <v>59</v>
       </c>
       <c r="E23" s="96" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F23" s="30" t="s">
-        <v>87</v>
+        <v>65</v>
       </c>
       <c r="G23" s="86" t="s">
         <v>33</v>
       </c>
       <c r="H23" s="30" t="s">
-        <v>154</v>
-      </c>
-      <c r="I23" s="86" t="s">
-        <v>33</v>
-      </c>
-      <c r="J23" s="86" t="s">
-        <v>33</v>
+        <v>153</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="J23" s="30" t="s">
+        <v>45</v>
       </c>
       <c r="K23" s="86" t="s">
         <v>46</v>
       </c>
-      <c r="L23" s="86" t="s">
-        <v>47</v>
-      </c>
-      <c r="M23" s="86" t="s">
-        <v>47</v>
-      </c>
-      <c r="N23" s="86" t="s">
-        <v>33</v>
+      <c r="L23" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="M23" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="N23" s="1" t="s">
+        <v>107</v>
       </c>
       <c r="O23" s="1" t="s">
         <v>45</v>
@@ -4396,17 +4453,17 @@
       <c r="P23" s="86" t="s">
         <v>180</v>
       </c>
-      <c r="Q23" s="86" t="s">
-        <v>33</v>
-      </c>
-      <c r="R23" s="30" t="s">
-        <v>111</v>
+      <c r="Q23" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="R23" s="1" t="s">
+        <v>110</v>
       </c>
       <c r="S23" s="30" t="s">
         <v>209</v>
       </c>
       <c r="T23" s="30" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="U23" s="1" t="s">
         <v>116</v>
@@ -4419,16 +4476,16 @@
       </c>
       <c r="X23" s="3"/>
     </row>
-    <row r="24" spans="1:24" ht="67.5">
+    <row r="24" spans="2:24" ht="94.5">
       <c r="B24" s="108"/>
-      <c r="C24" s="105" t="s">
-        <v>216</v>
+      <c r="C24" s="92" t="s">
+        <v>198</v>
       </c>
       <c r="D24" s="84" t="s">
-        <v>171</v>
-      </c>
-      <c r="E24" s="97" t="s">
-        <v>184</v>
+        <v>12</v>
+      </c>
+      <c r="E24" s="96" t="s">
+        <v>191</v>
       </c>
       <c r="F24" s="30" t="s">
         <v>87</v>
@@ -4472,8 +4529,8 @@
       <c r="S24" s="30" t="s">
         <v>209</v>
       </c>
-      <c r="T24" s="1" t="s">
-        <v>212</v>
+      <c r="T24" s="30" t="s">
+        <v>210</v>
       </c>
       <c r="U24" s="1" t="s">
         <v>116</v>
@@ -4481,21 +4538,21 @@
       <c r="V24" s="86" t="s">
         <v>33</v>
       </c>
-      <c r="W24" s="86" t="s">
-        <v>33</v>
+      <c r="W24" s="1" t="s">
+        <v>128</v>
       </c>
       <c r="X24" s="3"/>
     </row>
-    <row r="25" spans="1:24" ht="67.5">
+    <row r="25" spans="2:24" ht="67.5">
       <c r="B25" s="108"/>
       <c r="C25" s="105" t="s">
         <v>216</v>
       </c>
       <c r="D25" s="84" t="s">
-        <v>217</v>
+        <v>171</v>
       </c>
       <c r="E25" s="97" t="s">
-        <v>218</v>
+        <v>184</v>
       </c>
       <c r="F25" s="30" t="s">
         <v>87</v>
@@ -4539,8 +4596,8 @@
       <c r="S25" s="30" t="s">
         <v>209</v>
       </c>
-      <c r="T25" s="30" t="s">
-        <v>219</v>
+      <c r="T25" s="1" t="s">
+        <v>212</v>
       </c>
       <c r="U25" s="1" t="s">
         <v>116</v>
@@ -4553,25 +4610,25 @@
       </c>
       <c r="X25" s="3"/>
     </row>
-    <row r="26" spans="1:24" ht="67.5">
+    <row r="26" spans="2:24" ht="67.5">
       <c r="B26" s="108"/>
-      <c r="C26" s="92" t="s">
-        <v>198</v>
+      <c r="C26" s="105" t="s">
+        <v>216</v>
       </c>
       <c r="D26" s="84" t="s">
-        <v>94</v>
-      </c>
-      <c r="E26" s="100" t="s">
-        <v>192</v>
+        <v>217</v>
+      </c>
+      <c r="E26" s="97" t="s">
+        <v>218</v>
       </c>
       <c r="F26" s="30" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="G26" s="86" t="s">
         <v>33</v>
       </c>
       <c r="H26" s="30" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I26" s="86" t="s">
         <v>33</v>
@@ -4601,30 +4658,32 @@
         <v>33</v>
       </c>
       <c r="R26" s="30" t="s">
-        <v>84</v>
+        <v>111</v>
       </c>
       <c r="S26" s="30" t="s">
         <v>209</v>
       </c>
-      <c r="T26" s="1"/>
+      <c r="T26" s="30" t="s">
+        <v>219</v>
+      </c>
       <c r="U26" s="1" t="s">
         <v>116</v>
       </c>
       <c r="V26" s="86" t="s">
         <v>33</v>
       </c>
-      <c r="W26" s="1" t="s">
-        <v>128</v>
+      <c r="W26" s="86" t="s">
+        <v>33</v>
       </c>
       <c r="X26" s="3"/>
     </row>
-    <row r="27" spans="1:24" ht="67.5">
-      <c r="B27" s="109"/>
+    <row r="27" spans="2:24" ht="67.5">
+      <c r="B27" s="108"/>
       <c r="C27" s="92" t="s">
         <v>198</v>
       </c>
       <c r="D27" s="84" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E27" s="100" t="s">
         <v>192</v>
@@ -4636,7 +4695,7 @@
         <v>33</v>
       </c>
       <c r="H27" s="30" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I27" s="86" t="s">
         <v>33</v>
@@ -4683,283 +4742,362 @@
       </c>
       <c r="X27" s="3"/>
     </row>
-    <row r="28" spans="1:24" ht="41.25" thickBot="1">
-      <c r="B28" s="103" t="s">
+    <row r="28" spans="2:24" ht="67.5">
+      <c r="B28" s="109"/>
+      <c r="C28" s="92" t="s">
+        <v>198</v>
+      </c>
+      <c r="D28" s="84" t="s">
+        <v>95</v>
+      </c>
+      <c r="E28" s="100" t="s">
+        <v>192</v>
+      </c>
+      <c r="F28" s="30" t="s">
+        <v>96</v>
+      </c>
+      <c r="G28" s="86" t="s">
+        <v>33</v>
+      </c>
+      <c r="H28" s="30" t="s">
+        <v>156</v>
+      </c>
+      <c r="I28" s="86" t="s">
+        <v>33</v>
+      </c>
+      <c r="J28" s="86" t="s">
+        <v>33</v>
+      </c>
+      <c r="K28" s="86" t="s">
+        <v>46</v>
+      </c>
+      <c r="L28" s="86" t="s">
+        <v>47</v>
+      </c>
+      <c r="M28" s="86" t="s">
+        <v>47</v>
+      </c>
+      <c r="N28" s="86" t="s">
+        <v>33</v>
+      </c>
+      <c r="O28" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="P28" s="86" t="s">
+        <v>180</v>
+      </c>
+      <c r="Q28" s="86" t="s">
+        <v>33</v>
+      </c>
+      <c r="R28" s="30" t="s">
+        <v>84</v>
+      </c>
+      <c r="S28" s="30" t="s">
+        <v>209</v>
+      </c>
+      <c r="T28" s="1"/>
+      <c r="U28" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="V28" s="86" t="s">
+        <v>33</v>
+      </c>
+      <c r="W28" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="X28" s="3"/>
+    </row>
+    <row r="29" spans="2:24" ht="41.25" thickBot="1">
+      <c r="B29" s="103" t="s">
         <v>200</v>
       </c>
-      <c r="C28" s="95" t="s">
+      <c r="C29" s="95" t="s">
         <v>13</v>
       </c>
-      <c r="D28" s="85" t="s">
+      <c r="D29" s="85" t="s">
         <v>13</v>
       </c>
-      <c r="E28" s="98" t="s">
+      <c r="E29" s="98" t="s">
         <v>185</v>
       </c>
-      <c r="F28" s="71" t="s">
+      <c r="F29" s="71" t="s">
         <v>21</v>
       </c>
-      <c r="G28" s="87" t="s">
-        <v>33</v>
-      </c>
-      <c r="H28" s="87" t="s">
+      <c r="G29" s="87" t="s">
+        <v>33</v>
+      </c>
+      <c r="H29" s="87" t="s">
         <v>85</v>
       </c>
-      <c r="I28" s="87" t="s">
-        <v>33</v>
-      </c>
-      <c r="J28" s="87" t="s">
-        <v>33</v>
-      </c>
-      <c r="K28" s="87" t="s">
+      <c r="I29" s="87" t="s">
+        <v>33</v>
+      </c>
+      <c r="J29" s="87" t="s">
+        <v>33</v>
+      </c>
+      <c r="K29" s="87" t="s">
         <v>46</v>
       </c>
-      <c r="L28" s="87" t="s">
+      <c r="L29" s="87" t="s">
         <v>47</v>
       </c>
-      <c r="M28" s="87" t="s">
+      <c r="M29" s="87" t="s">
         <v>47</v>
       </c>
-      <c r="N28" s="87" t="s">
-        <v>33</v>
-      </c>
-      <c r="O28" s="87" t="s">
-        <v>33</v>
-      </c>
-      <c r="P28" s="86" t="s">
+      <c r="N29" s="87" t="s">
+        <v>33</v>
+      </c>
+      <c r="O29" s="87" t="s">
+        <v>33</v>
+      </c>
+      <c r="P29" s="86" t="s">
         <v>181</v>
       </c>
-      <c r="Q28" s="87" t="s">
-        <v>33</v>
-      </c>
-      <c r="R28" s="6" t="s">
+      <c r="Q29" s="87" t="s">
+        <v>33</v>
+      </c>
+      <c r="R29" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="S28" s="71" t="s">
+      <c r="S29" s="71" t="s">
         <v>209</v>
       </c>
-      <c r="T28" s="6"/>
-      <c r="U28" s="6" t="s">
+      <c r="T29" s="6"/>
+      <c r="U29" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="V28" s="87" t="s">
-        <v>33</v>
-      </c>
-      <c r="W28" s="6" t="s">
+      <c r="V29" s="87" t="s">
+        <v>33</v>
+      </c>
+      <c r="W29" s="6" t="s">
         <v>130</v>
       </c>
-      <c r="X28" s="7"/>
-    </row>
-    <row r="32" spans="1:24">
-      <c r="A32" s="106" t="s">
+      <c r="X29" s="7"/>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" s="106" t="s">
         <v>223</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B33" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
-      <c r="B33" s="60" t="s">
+    <row r="34" spans="1:3">
+      <c r="B34" s="60" t="s">
         <v>139</v>
       </c>
-      <c r="C33" s="60"/>
-    </row>
-    <row r="35" spans="1:3">
-      <c r="A35" s="106" t="s">
+      <c r="C34" s="60"/>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" s="106" t="s">
         <v>224</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B36" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="36" spans="1:3">
-      <c r="B36" s="60" t="s">
+    <row r="37" spans="1:3">
+      <c r="B37" s="60" t="s">
         <v>138</v>
       </c>
-      <c r="C36" s="60"/>
-    </row>
-    <row r="38" spans="1:3">
-      <c r="A38" s="106" t="s">
+      <c r="C37" s="60"/>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" s="106" t="s">
         <v>225</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B39" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="39" spans="1:3">
-      <c r="B39" s="60" t="s">
+    <row r="40" spans="1:3">
+      <c r="B40" s="60" t="s">
         <v>137</v>
       </c>
-      <c r="C39" s="60"/>
-    </row>
-    <row r="41" spans="1:3">
-      <c r="A41" s="106" t="s">
+      <c r="C40" s="60"/>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42" s="106" t="s">
         <v>226</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B42" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="42" spans="1:3">
-      <c r="B42" s="60" t="s">
+    <row r="43" spans="1:3">
+      <c r="B43" s="60" t="s">
         <v>136</v>
       </c>
-      <c r="C42" s="60"/>
-    </row>
-    <row r="44" spans="1:3">
-      <c r="A44" s="106" t="s">
+      <c r="C43" s="60"/>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="A45" s="106" t="s">
         <v>227</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B45" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="45" spans="1:3">
-      <c r="B45" s="61" t="s">
+    <row r="46" spans="1:3">
+      <c r="B46" s="61" t="s">
         <v>131</v>
       </c>
-      <c r="C45" s="61"/>
-    </row>
-    <row r="46" spans="1:3">
-      <c r="B46" s="60" t="s">
-        <v>135</v>
-      </c>
-      <c r="C46" s="60"/>
+      <c r="C46" s="61"/>
     </row>
     <row r="47" spans="1:3">
       <c r="B47" s="60" t="s">
+        <v>135</v>
+      </c>
+      <c r="C47" s="60"/>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="B48" s="60" t="s">
         <v>140</v>
       </c>
-      <c r="C47" s="60"/>
-    </row>
-    <row r="49" spans="1:3">
-      <c r="A49" s="106" t="s">
+      <c r="C48" s="60"/>
+    </row>
+    <row r="50" spans="1:3">
+      <c r="A50" s="106" t="s">
         <v>228</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B50" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="50" spans="1:3">
-      <c r="B50" s="60" t="s">
+    <row r="51" spans="1:3">
+      <c r="B51" s="60" t="s">
         <v>158</v>
       </c>
-      <c r="C50" s="60"/>
-    </row>
-    <row r="52" spans="1:3">
-      <c r="A52" s="106" t="s">
+      <c r="C51" s="60"/>
+    </row>
+    <row r="53" spans="1:3">
+      <c r="A53" s="106" t="s">
         <v>229</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B53" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="53" spans="1:3">
-      <c r="B53" s="60" t="s">
+    <row r="54" spans="1:3">
+      <c r="B54" s="60" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="55" spans="1:3">
-      <c r="A55" s="106" t="s">
+    <row r="56" spans="1:3">
+      <c r="A56" s="106" t="s">
         <v>230</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B56" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="56" spans="1:3">
-      <c r="B56" s="60" t="s">
+    <row r="57" spans="1:3">
+      <c r="B57" s="60" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="58" spans="1:3">
-      <c r="A58" s="106" t="s">
+    <row r="59" spans="1:3">
+      <c r="A59" s="106" t="s">
         <v>231</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B59" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="59" spans="1:3">
-      <c r="B59" s="60" t="s">
+    <row r="60" spans="1:3">
+      <c r="B60" s="60" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="61" spans="1:3">
-      <c r="A61" s="106" t="s">
+    <row r="62" spans="1:3">
+      <c r="A62" s="106" t="s">
         <v>232</v>
       </c>
-      <c r="B61" t="s">
+      <c r="B62" t="s">
         <v>213</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3">
-      <c r="B62" s="60" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="63" spans="1:3">
       <c r="B63" s="60" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3">
+      <c r="B64" s="60" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="65" spans="1:2">
-      <c r="A65" s="106" t="s">
+    <row r="66" spans="1:2">
+      <c r="A66" s="106" t="s">
         <v>233</v>
       </c>
-      <c r="B65" t="s">
+      <c r="B66" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="66" spans="1:2">
-      <c r="B66" s="60" t="s">
+    <row r="67" spans="1:2">
+      <c r="B67" s="60" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="68" spans="1:2">
-      <c r="A68" s="106" t="s">
+    <row r="69" spans="1:2">
+      <c r="A69" s="106" t="s">
+        <v>242</v>
+      </c>
+      <c r="B69" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2">
+      <c r="B70" s="60" t="s">
         <v>244</v>
       </c>
-      <c r="B68" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2">
-      <c r="B69" s="60" t="s">
-        <v>246</v>
+    </row>
+    <row r="72" spans="1:2">
+      <c r="A72" s="106" t="s">
+        <v>251</v>
+      </c>
+      <c r="B72" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2">
+      <c r="B73" s="60" t="s">
+        <v>253</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B8:B27"/>
+    <mergeCell ref="B8:B28"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <hyperlinks>
-    <hyperlink ref="B45" r:id="rId1"/>
-    <hyperlink ref="B46" r:id="rId2"/>
-    <hyperlink ref="B42" r:id="rId3"/>
-    <hyperlink ref="B39" r:id="rId4"/>
-    <hyperlink ref="B36" r:id="rId5"/>
-    <hyperlink ref="B33" r:id="rId6"/>
-    <hyperlink ref="B47" r:id="rId7"/>
-    <hyperlink ref="B50" r:id="rId8"/>
-    <hyperlink ref="B53" r:id="rId9"/>
-    <hyperlink ref="B56" r:id="rId10"/>
-    <hyperlink ref="B59" r:id="rId11"/>
-    <hyperlink ref="B62" r:id="rId12"/>
-    <hyperlink ref="B63" r:id="rId13"/>
-    <hyperlink ref="B66" r:id="rId14"/>
-    <hyperlink ref="B69" r:id="rId15"/>
+    <hyperlink ref="B46" r:id="rId1"/>
+    <hyperlink ref="B47" r:id="rId2"/>
+    <hyperlink ref="B43" r:id="rId3"/>
+    <hyperlink ref="B40" r:id="rId4"/>
+    <hyperlink ref="B37" r:id="rId5"/>
+    <hyperlink ref="B34" r:id="rId6"/>
+    <hyperlink ref="B48" r:id="rId7"/>
+    <hyperlink ref="B51" r:id="rId8"/>
+    <hyperlink ref="B54" r:id="rId9"/>
+    <hyperlink ref="B57" r:id="rId10"/>
+    <hyperlink ref="B60" r:id="rId11"/>
+    <hyperlink ref="B63" r:id="rId12"/>
+    <hyperlink ref="B64" r:id="rId13"/>
+    <hyperlink ref="B67" r:id="rId14"/>
+    <hyperlink ref="B70" r:id="rId15"/>
+    <hyperlink ref="B73" r:id="rId16"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="8" scale="42" orientation="landscape" horizontalDpi="4294967293" r:id="rId16"/>
-  <drawing r:id="rId17"/>
-  <legacyDrawing r:id="rId18"/>
+  <pageSetup paperSize="8" scale="42" orientation="landscape" horizontalDpi="4294967293" r:id="rId17"/>
+  <drawing r:id="rId18"/>
+  <legacyDrawing r:id="rId19"/>
   <oleObjects>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <oleObject progId="Visio.Drawing.15" shapeId="4097" r:id="rId19">
-          <objectPr defaultSize="0" autoPict="0" r:id="rId20">
+        <oleObject progId="Visio.Drawing.15" shapeId="4097" r:id="rId20">
+          <objectPr defaultSize="0" autoPict="0" r:id="rId21">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>1</xdr:col>
@@ -4978,7 +5116,7 @@
         </oleObject>
       </mc:Choice>
       <mc:Fallback>
-        <oleObject progId="Visio.Drawing.15" shapeId="4097" r:id="rId19"/>
+        <oleObject progId="Visio.Drawing.15" shapeId="4097" r:id="rId20"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </oleObjects>

</xml_diff>

<commit_message>
MSX0 Booster0/3 → MSX Booster0/3
</commit_message>
<xml_diff>
--- a/msx3gen/files/msx_gen3.xlsx
+++ b/msx3gen/files/msx_gen3.xlsx
@@ -1703,14 +1703,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>MSX0 Booster0</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>MSX0 Booster3</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>MSX0 Booster0 自体が
 カートリッジ。
 MSXのカートリッジスロット
@@ -1774,6 +1766,14 @@
   </si>
   <si>
     <t>https://x.com/nishikazuhiko/status/1695642892734521625</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>MSX Booster3</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>MSX Booster0</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -3304,10 +3304,10 @@
   <dimension ref="A3:X73"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="7" topLeftCell="Q42" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="7" topLeftCell="E8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="R71" sqref="R71"/>
+      <selection pane="bottomRight" activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -3948,7 +3948,7 @@
         <v>235</v>
       </c>
       <c r="D16" s="84" t="s">
-        <v>245</v>
+        <v>253</v>
       </c>
       <c r="E16" s="97" t="s">
         <v>183</v>
@@ -3981,7 +3981,7 @@
         <v>241</v>
       </c>
       <c r="O16" s="30" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="P16" s="86" t="s">
         <v>33</v>
@@ -3996,7 +3996,7 @@
         <v>166</v>
       </c>
       <c r="T16" s="30" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="U16" s="1" t="s">
         <v>165</v>
@@ -4009,25 +4009,25 @@
       </c>
       <c r="X16" s="3"/>
     </row>
-    <row r="17" spans="2:24" ht="54">
+    <row r="17" spans="2:24" ht="67.5">
       <c r="B17" s="108"/>
       <c r="C17" s="102" t="s">
         <v>235</v>
       </c>
       <c r="D17" s="84" t="s">
-        <v>246</v>
+        <v>252</v>
       </c>
       <c r="E17" s="97" t="s">
         <v>183</v>
       </c>
       <c r="F17" s="30" t="s">
-        <v>236</v>
+        <v>87</v>
       </c>
       <c r="G17" s="1" t="s">
         <v>237</v>
       </c>
       <c r="H17" s="30" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="I17" s="1" t="s">
         <v>239</v>
@@ -4045,10 +4045,10 @@
         <v>42</v>
       </c>
       <c r="N17" s="1" t="s">
-        <v>241</v>
+        <v>247</v>
       </c>
       <c r="O17" s="30" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="P17" s="86" t="s">
         <v>33</v>
@@ -5055,15 +5055,15 @@
     </row>
     <row r="72" spans="1:2">
       <c r="A72" s="106" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="B72" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="73" spans="1:2">
       <c r="B73" s="60" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
   </sheetData>

</xml_diff>